<commit_message>
finish patient list e2e some test are flaky, have to re-check
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="67">
   <si>
     <t xml:space="preserve">Clinic Mangement System Functional Test Cases (http://localhost:8000)</t>
   </si>
@@ -800,8 +800,8 @@
   </sheetPr>
   <dimension ref="B3:I9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -959,8 +959,8 @@
   </sheetPr>
   <dimension ref="B3:I8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1017,7 +1017,9 @@
       <c r="F6" s="21"/>
       <c r="G6" s="21"/>
       <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
+      <c r="I6" s="15" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="21" t="n">
@@ -1031,7 +1033,9 @@
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
       <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
+      <c r="I7" s="15" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="21" t="n">
@@ -1045,7 +1049,9 @@
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
       <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
+      <c r="I8" s="15" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>